<commit_message>
Update of 2.5 excel sheet
</commit_message>
<xml_diff>
--- a/futurelearn/Mastering Excel Pivot Tables/New_files/2.5 Adding records using a dynamic data source.xlsx
+++ b/futurelearn/Mastering Excel Pivot Tables/New_files/2.5 Adding records using a dynamic data source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wdmycloud\Danielle\Documents\DOC Office\Projects\Adelaide Uni\Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projects\Adelaide Uni\Pivot Table Course Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863B4A0F-4DC4-4BD5-B93F-4BA4FEC570C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4511BCD2-CA4D-4801-8CC6-AE4CE5C885FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30150" yWindow="1515" windowWidth="24225" windowHeight="13995" firstSheet="1" activeTab="1" xr2:uid="{41F9AD93-36FC-4D3E-8863-4F99BF54BC61}"/>
+    <workbookView xWindow="28680" yWindow="960" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{41F9AD93-36FC-4D3E-8863-4F99BF54BC61}"/>
   </bookViews>
   <sheets>
     <sheet name="List Data" sheetId="2" state="veryHidden" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="703">
   <si>
     <t>Thumb</t>
   </si>
@@ -2156,21 +2156,6 @@
   </si>
   <si>
     <t>Restricted Work Injury</t>
-  </si>
-  <si>
-    <t>CPM2288</t>
-  </si>
-  <si>
-    <t>Alby Roberts</t>
-  </si>
-  <si>
-    <t>Struck thumb with hammer</t>
-  </si>
-  <si>
-    <t>Driven to hospital ER for treatment</t>
-  </si>
-  <si>
-    <t>thumb</t>
   </si>
 </sst>
 </file>
@@ -2372,7 +2357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2486,7 +2471,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2616,9 +2600,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2656,7 +2640,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2762,7 +2746,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2904,7 +2888,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3832,14 +3816,14 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:O181"/>
+  <dimension ref="A1:O180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="G18" sqref="G18"/>
       <selection pane="topRight" activeCell="G18" sqref="G18"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K164" sqref="K164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11137,69 +11121,22 @@
       <c r="N180" s="9"/>
       <c r="O180" s="9"/>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A181" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="B181" s="41">
-        <v>45017</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="D181" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="F181" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G181" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H181" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I181" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J181" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="K181" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L181" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M181" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="N181" s="1">
-        <v>0</v>
-      </c>
-      <c r="O181" s="1">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:O180" xr:uid="{9C8234ED-84F1-4893-A8D8-9A88F596E03E}"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D184:D1048576 D1:D182" xr:uid="{2AE9394A-88BD-4259-89F3-26685B85982A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D183:D1048576 D1:D181" xr:uid="{2AE9394A-88BD-4259-89F3-26685B85982A}">
       <formula1>rngProjects</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H182 H184:H1048576" xr:uid="{4CCCB194-367F-4B73-AD49-5460713EECF2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H183:H1048576 H1:H181" xr:uid="{4CCCB194-367F-4B73-AD49-5460713EECF2}">
       <formula1>rngCauseOfInjury</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I182 I184:I1048576" xr:uid="{2D156E48-F8D4-4369-9D96-6F8D709FDBEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I183:I1048576 I1:I181" xr:uid="{2D156E48-F8D4-4369-9D96-6F8D709FDBEC}">
       <formula1>rngIncidentType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K182 K184:K1048576" xr:uid="{7D651E6D-5AB2-4FED-9AC9-9DA8DA34CCB4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K183:K1048576 K1:K181" xr:uid="{7D651E6D-5AB2-4FED-9AC9-9DA8DA34CCB4}">
       <formula1>rngInjuryType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L182 L184:L1048576" xr:uid="{38D256A6-A840-4E99-9A9F-1E02DEB63558}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L183:L1048576 L1:L181" xr:uid="{38D256A6-A840-4E99-9A9F-1E02DEB63558}">
       <formula1>rngBodyLocationGeneral</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{DB07510F-B595-4DCA-9649-0A44C00C3A27}">

</xml_diff>